<commit_message>
Update training experiments spreadsheet with latest experiments
</commit_message>
<xml_diff>
--- a/docs/experiments/Training_Experiments.xlsx
+++ b/docs/experiments/Training_Experiments.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
   <si>
     <t>EfficientDet</t>
   </si>
@@ -235,6 +235,31 @@
   </si>
   <si>
     <t>efficientdet_b0_20220520_104949.h5</t>
+  </si>
+  <si>
+    <t>Stratified (ID); Exclude cell accu; Sliced 384x384</t>
+  </si>
+  <si>
+    <t>anchor_box_ratios: [1, 0.5, 2]
+anchor_box_scales: [0.4, 0.496, 0.625]
+LR Reduce Patience: 2
+LR Min Delta: 0.001
+LR Reduce Factor: 0.1</t>
+  </si>
+  <si>
+    <t>100 (22)</t>
+  </si>
+  <si>
+    <t>efficientdet_b0_20220607_111240.h5</t>
+  </si>
+  <si>
+    <t>Stratified (ID); Sliced 384x384</t>
+  </si>
+  <si>
+    <t>100 (28)</t>
+  </si>
+  <si>
+    <t>efficientdet_b0_20220607_132616.h5</t>
   </si>
 </sst>
 </file>
@@ -2232,19 +2257,45 @@
       <c r="Z31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="7"/>
+      <c r="A32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="G32" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0.9365</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0.9365</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0.9365</v>
+      </c>
+      <c r="L32" s="12">
+        <v>18.4</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
@@ -2260,19 +2311,42 @@
       <c r="Z32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="7"/>
+      <c r="A33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="G33" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0.936</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.601</v>
+      </c>
+      <c r="J33" s="11">
+        <v>0.7685</v>
+      </c>
+      <c r="K33" s="11">
+        <v>0.9268</v>
+      </c>
+      <c r="L33" s="12">
+        <v>16.0</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
@@ -29308,11 +29382,12 @@
       <c r="Z998" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>